<commit_message>
add consump to stock
</commit_message>
<xml_diff>
--- a/database/industries/folad/faspa/product/monthly.xlsx
+++ b/database/industries/folad/faspa/product/monthly.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\folad\faspa\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\folad\faspa\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6F3C56-3C8A-4371-BDDB-44AABEF67D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="82">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -202,13 +201,7 @@
     <t>ورق,بندل,کلاف</t>
   </si>
   <si>
-    <t>لوله های گازی و صنعتی</t>
-  </si>
-  <si>
     <t>محصولات اجرتی</t>
-  </si>
-  <si>
-    <t>انواع لوله گازی و صنعتی</t>
   </si>
   <si>
     <t>محصول صادراتی</t>
@@ -270,11 +263,14 @@
   <si>
     <t>نرخ درآمد ارایه خدمات</t>
   </si>
+  <si>
+    <t>لوله</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,10 +736,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1891,7 +1889,7 @@
     </row>
     <row r="14" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>56</v>
@@ -2050,7 +2048,7 @@
     </row>
     <row r="15" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>56</v>
@@ -2209,7 +2207,7 @@
     </row>
     <row r="16" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>56</v>
@@ -2368,7 +2366,7 @@
     </row>
     <row r="17" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>56</v>
@@ -2527,10 +2525,10 @@
     </row>
     <row r="18" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
@@ -2686,7 +2684,7 @@
     </row>
     <row r="19" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>56</v>
@@ -2845,7 +2843,7 @@
     </row>
     <row r="20" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>56</v>
@@ -3004,7 +3002,7 @@
     </row>
     <row r="21" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -3061,7 +3059,7 @@
     </row>
     <row r="22" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>56</v>
@@ -3220,7 +3218,7 @@
     </row>
     <row r="23" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -3377,7 +3375,7 @@
     </row>
     <row r="24" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -3699,7 +3697,7 @@
     </row>
     <row r="28" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -3911,7 +3909,7 @@
     </row>
     <row r="30" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -4445,7 +4443,7 @@
     </row>
     <row r="34" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>56</v>
@@ -4604,7 +4602,7 @@
     </row>
     <row r="35" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>56</v>
@@ -4763,7 +4761,7 @@
     </row>
     <row r="36" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>56</v>
@@ -4922,7 +4920,7 @@
     </row>
     <row r="37" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>56</v>
@@ -5081,10 +5079,10 @@
     </row>
     <row r="38" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13" t="s">
@@ -5240,7 +5238,7 @@
     </row>
     <row r="39" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>56</v>
@@ -5399,7 +5397,7 @@
     </row>
     <row r="40" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>56</v>
@@ -5558,7 +5556,7 @@
     </row>
     <row r="41" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -5615,7 +5613,7 @@
     </row>
     <row r="42" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>56</v>
@@ -5774,7 +5772,7 @@
     </row>
     <row r="43" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -5931,7 +5929,7 @@
     </row>
     <row r="44" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -5988,7 +5986,7 @@
     </row>
     <row r="45" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>56</v>
@@ -6147,7 +6145,7 @@
     </row>
     <row r="46" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>56</v>
@@ -6306,7 +6304,7 @@
     </row>
     <row r="47" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -6463,7 +6461,7 @@
     </row>
     <row r="48" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
@@ -6785,7 +6783,7 @@
     </row>
     <row r="52" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -6997,7 +6995,7 @@
     </row>
     <row r="54" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -7057,7 +7055,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
@@ -7216,7 +7214,7 @@
         <v>58</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="13">
@@ -7375,7 +7373,7 @@
         <v>59</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11">
@@ -7531,10 +7529,10 @@
     </row>
     <row r="58" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B58" s="12" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="13">
@@ -7690,10 +7688,10 @@
     </row>
     <row r="59" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D59" s="11"/>
       <c r="E59" s="11">
@@ -7849,10 +7847,10 @@
     </row>
     <row r="60" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="13" t="s">
@@ -8008,10 +8006,10 @@
     </row>
     <row r="61" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="11" t="s">
@@ -8167,10 +8165,10 @@
     </row>
     <row r="62" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="13" t="s">
@@ -8326,10 +8324,10 @@
     </row>
     <row r="63" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="11" t="s">
@@ -8485,10 +8483,10 @@
     </row>
     <row r="64" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B64" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="13" t="s">
@@ -8644,7 +8642,7 @@
     </row>
     <row r="65" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
@@ -8701,10 +8699,10 @@
     </row>
     <row r="66" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="11" t="s">
@@ -8860,10 +8858,10 @@
     </row>
     <row r="67" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67" s="15" t="s">
@@ -9019,7 +9017,7 @@
     </row>
     <row r="68" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -9076,10 +9074,10 @@
     </row>
     <row r="69" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11" t="s">
@@ -9235,10 +9233,10 @@
     </row>
     <row r="70" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B70" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="13" t="s">
@@ -9394,10 +9392,10 @@
     </row>
     <row r="71" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="17" t="s">
@@ -9553,7 +9551,7 @@
     </row>
     <row r="72" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -9610,10 +9608,10 @@
     </row>
     <row r="73" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="11" t="s">
@@ -9769,7 +9767,7 @@
     </row>
     <row r="74" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
@@ -10091,7 +10089,7 @@
     </row>
     <row r="78" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B78" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -10303,7 +10301,7 @@
     </row>
     <row r="80" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
@@ -10363,7 +10361,7 @@
         <v>55</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="11" t="s">
@@ -10522,7 +10520,7 @@
         <v>58</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="13">
@@ -10681,7 +10679,7 @@
         <v>59</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D83" s="11"/>
       <c r="E83" s="11">
@@ -10837,10 +10835,10 @@
     </row>
     <row r="84" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B84" s="12" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="13">
@@ -10996,10 +10994,10 @@
     </row>
     <row r="85" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11">
@@ -11155,10 +11153,10 @@
     </row>
     <row r="86" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B86" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="13" t="s">
@@ -11314,10 +11312,10 @@
     </row>
     <row r="87" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11" t="s">
@@ -11473,10 +11471,10 @@
     </row>
     <row r="88" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B88" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="13" t="s">
@@ -11632,7 +11630,7 @@
     </row>
     <row r="89" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -11689,10 +11687,10 @@
     </row>
     <row r="90" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B90" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11" t="s">

</xml_diff>